<commit_message>
Improving model behavior and reducing dummies in the solves
</commit_message>
<xml_diff>
--- a/manual_additions/additional backbone input.xlsx
+++ b/manual_additions/additional backbone input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\manual_additions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1E3074-8A7D-4646-87E5-FB95BCF5480B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071A4385-0A65-44C4-9926-5603D73DEAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="p_gn" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="rngFuelPricesDeterministic">'[1]Commodity inputs and calcs'!$M$14:$P$21</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="51">
   <si>
     <t>Type</t>
   </si>
@@ -150,40 +150,52 @@
     <t>boundStart</t>
   </si>
   <si>
+    <t>BE00_ror</t>
+  </si>
+  <si>
+    <t>DE00_ror</t>
+  </si>
+  <si>
+    <t>ES00_ror</t>
+  </si>
+  <si>
+    <t>FR00_ror</t>
+  </si>
+  <si>
+    <t>LT00_ror</t>
+  </si>
+  <si>
+    <t>LV00_ror</t>
+  </si>
+  <si>
+    <t>NL00_ror</t>
+  </si>
+  <si>
+    <t>PL00_ror</t>
+  </si>
+  <si>
+    <t>UK00_ror</t>
+  </si>
+  <si>
     <t>DE00_psOpen</t>
   </si>
   <si>
+    <t>ES00_psOpen</t>
+  </si>
+  <si>
     <t>FR00_psOpen</t>
   </si>
   <si>
     <t>PL00_psOpen</t>
   </si>
   <si>
-    <t>DE00_psClosed</t>
-  </si>
-  <si>
-    <t>FR00_psClosed</t>
-  </si>
-  <si>
-    <t>LT00_psClosed</t>
-  </si>
-  <si>
-    <t>PL00_psClosed</t>
-  </si>
-  <si>
-    <t>UK00_psClosed</t>
-  </si>
-  <si>
     <t>DE00_reservoir</t>
   </si>
   <si>
+    <t>ES00_reservoir</t>
+  </si>
+  <si>
     <t>PL00_reservoir</t>
-  </si>
-  <si>
-    <t>PL00_batterystor</t>
-  </si>
-  <si>
-    <t>UK00_batterystor</t>
   </si>
 </sst>
 </file>
@@ -683,18 +695,18 @@
       <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6:E26"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
     <col min="4" max="4" width="4" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -708,7 +720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -722,7 +734,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -733,7 +745,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -747,35 +759,35 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
-        <v>35</v>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D6"/>
       <c r="E6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
-        <v>36</v>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D7"/>
       <c r="E7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D8"/>
@@ -783,11 +795,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D9"/>
@@ -795,1465 +807,1339 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
-        <v>22</v>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D10"/>
       <c r="E10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" t="s">
-        <v>37</v>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D11"/>
       <c r="E11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
-        <v>38</v>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="D12"/>
       <c r="E12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
-      </c>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D13"/>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D14"/>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D15"/>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D16"/>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>43</v>
-      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17"/>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18"/>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D19"/>
-      <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
-        <v>44</v>
-      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D20"/>
-      <c r="E20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s">
-        <v>25</v>
-      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D21"/>
-      <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
-        <v>26</v>
-      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D22"/>
-      <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" t="s">
-        <v>27</v>
-      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D23"/>
-      <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" t="s">
-        <v>29</v>
-      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D24"/>
-      <c r="E24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" t="s">
-        <v>45</v>
-      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D25"/>
-      <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" t="s">
-        <v>46</v>
-      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D26"/>
-      <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D27"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D28"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D29"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D30"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D31"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D32"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D34"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D37"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D38"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D39"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D40"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D41"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D42"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D43"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D44"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D45"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D46"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D47"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D48"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D49"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D50"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D51"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D52"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D53"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D54"/>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D55"/>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D56"/>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D57"/>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D58"/>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D59"/>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D60"/>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D61"/>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D62"/>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D63"/>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D64"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D65"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D66"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D67"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D68"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D69"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D70"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D71"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D72"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D73"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D74"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D75"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D76"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D77"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D78"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D79"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D80"/>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D81"/>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D82"/>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D83"/>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D84"/>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D85"/>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D86"/>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D87"/>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D88"/>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D89"/>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D90"/>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D91"/>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D92"/>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D93"/>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D94"/>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D95"/>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D96"/>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D97"/>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D98"/>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D99"/>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D100"/>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D101"/>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D102"/>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D103"/>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D104"/>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D105"/>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D106"/>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D107"/>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D108"/>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D109"/>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D110"/>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D111"/>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D112"/>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D113"/>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D114"/>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D115"/>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D116"/>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D117"/>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D118"/>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D119"/>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D120"/>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D121"/>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D122"/>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D123"/>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D124"/>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D125"/>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D126"/>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D127"/>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D128"/>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D129"/>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D130"/>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D131"/>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D132"/>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D133"/>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D134"/>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D135"/>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D136"/>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D137"/>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D138"/>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D139"/>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D140"/>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D141"/>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D142"/>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D143"/>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D144"/>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D145"/>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D146"/>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D147"/>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D148"/>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D149"/>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D150"/>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D151"/>
     </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D152"/>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D153"/>
     </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D154"/>
     </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D155"/>
     </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D156"/>
     </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D157"/>
     </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D158"/>
     </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D159"/>
     </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D160"/>
     </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D161"/>
     </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D162"/>
     </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D163"/>
     </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D164"/>
     </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D165"/>
     </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D166"/>
     </row>
-    <row r="167" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D167"/>
     </row>
-    <row r="168" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D168"/>
     </row>
-    <row r="169" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D169"/>
     </row>
-    <row r="170" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D170"/>
     </row>
-    <row r="171" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D171"/>
     </row>
-    <row r="172" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D172"/>
     </row>
-    <row r="173" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D173"/>
     </row>
-    <row r="174" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D174"/>
     </row>
-    <row r="175" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D175"/>
     </row>
-    <row r="176" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D176"/>
     </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D177"/>
     </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D178"/>
     </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D179"/>
     </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D180"/>
     </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D181"/>
     </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D182"/>
     </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D183"/>
     </row>
-    <row r="184" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D184"/>
     </row>
-    <row r="185" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D185"/>
     </row>
-    <row r="186" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D186"/>
     </row>
-    <row r="187" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D187"/>
     </row>
-    <row r="188" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D188"/>
     </row>
-    <row r="189" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D189"/>
     </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D190"/>
     </row>
-    <row r="191" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D191"/>
     </row>
-    <row r="192" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D192"/>
     </row>
-    <row r="193" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D193"/>
     </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D194"/>
     </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D195"/>
     </row>
-    <row r="196" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D196"/>
     </row>
-    <row r="197" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D197"/>
     </row>
-    <row r="198" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D198"/>
     </row>
-    <row r="199" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D199"/>
     </row>
-    <row r="200" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D200"/>
     </row>
-    <row r="201" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D201"/>
     </row>
-    <row r="202" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D202"/>
     </row>
-    <row r="203" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D203"/>
     </row>
-    <row r="204" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D204"/>
     </row>
-    <row r="205" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D205"/>
     </row>
-    <row r="206" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D206"/>
     </row>
-    <row r="207" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D207"/>
     </row>
-    <row r="208" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D208"/>
     </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D209"/>
     </row>
-    <row r="210" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D210"/>
     </row>
-    <row r="211" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D211"/>
     </row>
-    <row r="212" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D212"/>
     </row>
-    <row r="213" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D213"/>
     </row>
-    <row r="214" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D214"/>
     </row>
-    <row r="215" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D215"/>
     </row>
-    <row r="216" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D216"/>
     </row>
-    <row r="217" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D217"/>
     </row>
-    <row r="218" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D218"/>
     </row>
-    <row r="219" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D219"/>
     </row>
-    <row r="220" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D220"/>
     </row>
-    <row r="221" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D221"/>
     </row>
-    <row r="222" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D222"/>
     </row>
-    <row r="223" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D223"/>
     </row>
-    <row r="224" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D224"/>
     </row>
-    <row r="225" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D225"/>
     </row>
-    <row r="226" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D226"/>
     </row>
-    <row r="227" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D227"/>
     </row>
-    <row r="228" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D228"/>
     </row>
-    <row r="229" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D229"/>
     </row>
-    <row r="230" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D230"/>
     </row>
-    <row r="231" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D231"/>
     </row>
-    <row r="232" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D232"/>
     </row>
-    <row r="233" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D233"/>
     </row>
-    <row r="234" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D234"/>
     </row>
-    <row r="235" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D235"/>
     </row>
-    <row r="236" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D236"/>
     </row>
-    <row r="237" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D237"/>
     </row>
-    <row r="238" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D238"/>
     </row>
-    <row r="239" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D239"/>
     </row>
-    <row r="240" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D240"/>
     </row>
-    <row r="241" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D241"/>
     </row>
-    <row r="242" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D242"/>
     </row>
-    <row r="243" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D243"/>
     </row>
-    <row r="244" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D244"/>
     </row>
-    <row r="245" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D245"/>
     </row>
-    <row r="246" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D246"/>
     </row>
-    <row r="247" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D247"/>
     </row>
-    <row r="248" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D248"/>
     </row>
-    <row r="249" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D249"/>
     </row>
-    <row r="250" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D250"/>
     </row>
-    <row r="251" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D251"/>
     </row>
-    <row r="252" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D252"/>
     </row>
-    <row r="253" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D253"/>
     </row>
-    <row r="254" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D254"/>
     </row>
-    <row r="255" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D255"/>
     </row>
-    <row r="256" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D256"/>
     </row>
-    <row r="257" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D257"/>
     </row>
-    <row r="258" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D258"/>
     </row>
-    <row r="259" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D259"/>
     </row>
-    <row r="260" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D260"/>
     </row>
-    <row r="261" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D261"/>
     </row>
-    <row r="262" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D262"/>
     </row>
-    <row r="263" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D263"/>
     </row>
-    <row r="264" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D264"/>
     </row>
-    <row r="265" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D265"/>
     </row>
-    <row r="266" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D266"/>
     </row>
-    <row r="267" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D267"/>
     </row>
-    <row r="268" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D268"/>
     </row>
-    <row r="269" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D269"/>
     </row>
-    <row r="270" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D270"/>
     </row>
-    <row r="271" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D271"/>
     </row>
-    <row r="272" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D272"/>
     </row>
-    <row r="273" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D273"/>
     </row>
-    <row r="274" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D274"/>
     </row>
-    <row r="275" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D275"/>
     </row>
-    <row r="276" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D276"/>
     </row>
-    <row r="277" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="277" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D277"/>
     </row>
-    <row r="278" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D278"/>
     </row>
-    <row r="279" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="279" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D279"/>
     </row>
-    <row r="280" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="280" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D280"/>
     </row>
-    <row r="281" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="281" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D281"/>
     </row>
-    <row r="282" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="282" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D282"/>
     </row>
-    <row r="283" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D283"/>
     </row>
-    <row r="284" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="284" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D284"/>
     </row>
-    <row r="285" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D285"/>
     </row>
-    <row r="286" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D286"/>
     </row>
-    <row r="287" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D287"/>
     </row>
-    <row r="288" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D288"/>
     </row>
-    <row r="289" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D289"/>
     </row>
-    <row r="290" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D290"/>
     </row>
-    <row r="291" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D291"/>
     </row>
-    <row r="292" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D292"/>
     </row>
-    <row r="293" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D293"/>
     </row>
-    <row r="294" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D294"/>
     </row>
-    <row r="295" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D295"/>
     </row>
-    <row r="296" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D296"/>
     </row>
-    <row r="297" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D297"/>
     </row>
-    <row r="298" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D298"/>
     </row>
-    <row r="299" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D299"/>
     </row>
-    <row r="300" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="300" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D300"/>
     </row>
-    <row r="301" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="301" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D301"/>
     </row>
-    <row r="302" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="302" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D302"/>
     </row>
-    <row r="303" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="303" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D303"/>
     </row>
-    <row r="304" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D304"/>
     </row>
-    <row r="305" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="305" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D305"/>
     </row>
-    <row r="306" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="306" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D306"/>
     </row>
-    <row r="307" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="307" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D307"/>
     </row>
-    <row r="308" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D308"/>
     </row>
-    <row r="309" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="309" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D309"/>
     </row>
-    <row r="310" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="310" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D310"/>
     </row>
-    <row r="311" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="311" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D311"/>
     </row>
-    <row r="312" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="312" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D312"/>
     </row>
-    <row r="313" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="313" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D313"/>
     </row>
-    <row r="314" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="314" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D314"/>
     </row>
-    <row r="315" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="315" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D315"/>
     </row>
-    <row r="316" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="316" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D316"/>
     </row>
-    <row r="317" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="317" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D317"/>
     </row>
-    <row r="318" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="318" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D318"/>
     </row>
-    <row r="319" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="319" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D319"/>
     </row>
-    <row r="320" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="320" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D320"/>
     </row>
-    <row r="321" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="321" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D321"/>
     </row>
-    <row r="322" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="322" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D322"/>
     </row>
-    <row r="323" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="323" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D323"/>
     </row>
-    <row r="324" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="324" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D324"/>
     </row>
-    <row r="325" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="325" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D325"/>
     </row>
-    <row r="326" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="326" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D326"/>
     </row>
-    <row r="327" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="327" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D327"/>
     </row>
-    <row r="328" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="328" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D328"/>
     </row>
-    <row r="329" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="329" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D329"/>
     </row>
-    <row r="330" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="330" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D330"/>
     </row>
-    <row r="331" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="331" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D331"/>
     </row>
-    <row r="332" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="332" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D332"/>
     </row>
-    <row r="333" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="333" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D333"/>
     </row>
-    <row r="334" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="334" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D334"/>
     </row>
-    <row r="335" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="335" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D335"/>
     </row>
-    <row r="336" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="336" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D336"/>
     </row>
-    <row r="337" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="337" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D337"/>
     </row>
-    <row r="338" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="338" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D338"/>
     </row>
-    <row r="339" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="339" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D339"/>
     </row>
-    <row r="340" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="340" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D340"/>
     </row>
-    <row r="341" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="341" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D341"/>
     </row>
-    <row r="342" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="342" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D342"/>
     </row>
-    <row r="343" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="343" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D343"/>
     </row>
-    <row r="344" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="344" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D344"/>
     </row>
-    <row r="345" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="345" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D345"/>
     </row>
-    <row r="346" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="346" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D346"/>
     </row>
-    <row r="347" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="347" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D347"/>
     </row>
-    <row r="348" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="348" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D348"/>
     </row>
-    <row r="349" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="349" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D349"/>
     </row>
-    <row r="350" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="350" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D350"/>
     </row>
-    <row r="351" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="351" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D351"/>
     </row>
-    <row r="352" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="352" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D352"/>
     </row>
-    <row r="353" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="353" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D353"/>
     </row>
-    <row r="354" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="354" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D354"/>
     </row>
-    <row r="355" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="355" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D355"/>
     </row>
-    <row r="356" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="356" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D356"/>
     </row>
-    <row r="357" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="357" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D357"/>
     </row>
-    <row r="358" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="358" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D358"/>
     </row>
-    <row r="359" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="359" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D359"/>
     </row>
-    <row r="360" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="360" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D360"/>
     </row>
-    <row r="361" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="361" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D361"/>
     </row>
-    <row r="362" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="362" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D362"/>
     </row>
-    <row r="363" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="363" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D363"/>
     </row>
-    <row r="364" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="364" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D364"/>
     </row>
-    <row r="365" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="365" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D365"/>
     </row>
-    <row r="366" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="366" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D366"/>
     </row>
-    <row r="367" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="367" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D367"/>
     </row>
-    <row r="368" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="368" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D368"/>
     </row>
-    <row r="369" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="369" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D369"/>
     </row>
-    <row r="370" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="370" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D370"/>
     </row>
-    <row r="371" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="371" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D371"/>
     </row>
-    <row r="372" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="372" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D372"/>
     </row>
-    <row r="373" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="373" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D373"/>
     </row>
-    <row r="374" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="374" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D374"/>
     </row>
-    <row r="375" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="375" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D375"/>
     </row>
-    <row r="376" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="376" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D376"/>
     </row>
-    <row r="377" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="377" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D377"/>
     </row>
-    <row r="378" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="378" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D378"/>
     </row>
-    <row r="379" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="379" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D379"/>
     </row>
-    <row r="380" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="380" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D380"/>
     </row>
-    <row r="381" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="381" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D381"/>
     </row>
-    <row r="382" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="382" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D382"/>
     </row>
-    <row r="383" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="383" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D383"/>
     </row>
-    <row r="384" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="384" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D384"/>
     </row>
-    <row r="385" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="385" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D385"/>
     </row>
-    <row r="386" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="386" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D386"/>
     </row>
-    <row r="387" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="387" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D387"/>
     </row>
-    <row r="388" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="388" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D388"/>
     </row>
-    <row r="389" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="389" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D389"/>
     </row>
-    <row r="390" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="390" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D390"/>
     </row>
-    <row r="391" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="391" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D391"/>
     </row>
-    <row r="392" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="392" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D392"/>
     </row>
-    <row r="393" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="393" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D393"/>
     </row>
-    <row r="394" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="394" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D394"/>
     </row>
-    <row r="395" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="395" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D395"/>
     </row>
-    <row r="396" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="396" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D396"/>
     </row>
-    <row r="397" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="397" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D397"/>
     </row>
-    <row r="398" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="398" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D398"/>
     </row>
-    <row r="399" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="399" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D399"/>
     </row>
-    <row r="400" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="400" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D400"/>
     </row>
-    <row r="401" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="401" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D401"/>
     </row>
-    <row r="402" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="402" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D402"/>
     </row>
-    <row r="403" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="403" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D403"/>
     </row>
-    <row r="404" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="404" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D404"/>
     </row>
-    <row r="405" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="405" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D405"/>
     </row>
-    <row r="406" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="406" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D406"/>
     </row>
-    <row r="407" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="407" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D407"/>
     </row>
-    <row r="408" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="408" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D408"/>
     </row>
-    <row r="409" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="409" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D409"/>
     </row>
-    <row r="410" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="410" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D410"/>
     </row>
-    <row r="411" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="411" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D411"/>
     </row>
-    <row r="412" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="412" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D412"/>
     </row>
-    <row r="413" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="413" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D413"/>
     </row>
-    <row r="414" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="414" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D414"/>
     </row>
-    <row r="415" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="415" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D415"/>
     </row>
-    <row r="416" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="416" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D416"/>
     </row>
-    <row r="417" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="417" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D417"/>
     </row>
-    <row r="418" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="418" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D418"/>
     </row>
-    <row r="419" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="419" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D419"/>
     </row>
-    <row r="420" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="420" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D420"/>
     </row>
-    <row r="421" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="421" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D421"/>
     </row>
-    <row r="422" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="422" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D422"/>
     </row>
-    <row r="423" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="423" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D423"/>
     </row>
-    <row r="424" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="424" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D424"/>
     </row>
-    <row r="425" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="425" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D425"/>
     </row>
-    <row r="426" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="426" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D426"/>
     </row>
-    <row r="427" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="427" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D427"/>
     </row>
-    <row r="428" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="428" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D428"/>
     </row>
-    <row r="429" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="429" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D429"/>
     </row>
-    <row r="430" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="430" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D430"/>
     </row>
-    <row r="431" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="431" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D431"/>
     </row>
-    <row r="432" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="432" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D432"/>
     </row>
-    <row r="433" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="433" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D433"/>
     </row>
-    <row r="434" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="434" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D434"/>
     </row>
-    <row r="435" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="435" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D435"/>
     </row>
-    <row r="436" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="436" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D436"/>
     </row>
-    <row r="437" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="437" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D437"/>
     </row>
-    <row r="438" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="438" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D438"/>
     </row>
-    <row r="439" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="439" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D439"/>
     </row>
-    <row r="440" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="440" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D440"/>
     </row>
-    <row r="441" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="441" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D441"/>
     </row>
-    <row r="442" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="442" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D442"/>
     </row>
-    <row r="443" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="443" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D443"/>
     </row>
-    <row r="444" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="444" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D444"/>
     </row>
-    <row r="445" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="445" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D445"/>
     </row>
   </sheetData>
@@ -2270,23 +2156,23 @@
   <dimension ref="A1:J505"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="5" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22:G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2303,7 +2189,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2317,7 +2203,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -2334,7 +2220,7 @@
       <c r="F4"/>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -2354,7 +2240,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
@@ -2374,7 +2260,7 @@
         <v>3300000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
@@ -2394,7 +2280,7 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
@@ -2414,7 +2300,7 @@
         <v>5500000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
@@ -2434,7 +2320,7 @@
         <v>12000000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
@@ -2454,7 +2340,7 @@
         <v>8500000</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
@@ -2474,7 +2360,7 @@
         <v>13000000</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>19</v>
       </c>
@@ -2494,7 +2380,7 @@
         <v>1800000</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
@@ -2514,7 +2400,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
@@ -2534,7 +2420,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
@@ -2554,7 +2440,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
@@ -2574,7 +2460,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
@@ -2594,7 +2480,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2614,7 +2500,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
@@ -2634,7 +2520,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
@@ -2654,7 +2540,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
@@ -2674,1613 +2560,1881 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="1" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
         <v>31</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
         <v>31</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23" s="1">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
         <v>31</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
-      <c r="F24" s="1">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
         <v>31</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="F25" s="1">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" t="s">
         <v>31</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26" s="1">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" t="s">
         <v>31</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
-      <c r="F27" s="1">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" t="s">
         <v>31</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="F28" s="1">
-        <v>1</v>
-      </c>
-      <c r="G28" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" t="s">
         <v>31</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29" s="1">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" t="s">
         <v>31</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
-      <c r="F30" s="1">
-        <v>1</v>
-      </c>
-      <c r="G30" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E32"/>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E34"/>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E35"/>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E36"/>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E37"/>
-    </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E38"/>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E39"/>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E40"/>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E41"/>
-    </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E42"/>
-    </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E43"/>
-    </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E44"/>
-    </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E45"/>
-    </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E46"/>
-    </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" t="s">
+        <v>31</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" t="s">
+        <v>31</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E47"/>
     </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E48"/>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E49"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E50"/>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E51"/>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E52"/>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E53"/>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E54"/>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E55"/>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E56"/>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E57"/>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E58"/>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E59"/>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E60"/>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E61"/>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E62"/>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E63"/>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E64"/>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E65"/>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E66"/>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E67"/>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E68"/>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E69"/>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E70"/>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E71"/>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E72"/>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E73"/>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E74"/>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E75"/>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E76"/>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E77"/>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E78"/>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E79"/>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E80"/>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E81"/>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E82"/>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E83"/>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E84"/>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E85"/>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E86"/>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E87"/>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E88"/>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E89"/>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E90"/>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E91"/>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E92"/>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E93"/>
     </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E94"/>
     </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E95"/>
     </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E96"/>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E97"/>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E98"/>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E99"/>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E100"/>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E101"/>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E102"/>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E103"/>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E104"/>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E105"/>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E106"/>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E107"/>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E108"/>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E109"/>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E110"/>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E111"/>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E112"/>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E113"/>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E114"/>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E115"/>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E116"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E117"/>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E118"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E119"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E120"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E121"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E122"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E123"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E124"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E125"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E126"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E127"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E128"/>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E129"/>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E130"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E131"/>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E132"/>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E133"/>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E134"/>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E135"/>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E136"/>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E137"/>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E138"/>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E139"/>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E140"/>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E141"/>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E142"/>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E143"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E144"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E145"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E146"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E147"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E148"/>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E149"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E150"/>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E151"/>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E152"/>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E153"/>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E154"/>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E155"/>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E156"/>
     </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E157"/>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E158"/>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E159"/>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E160"/>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E161"/>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E162"/>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E163"/>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E164"/>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E165"/>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E166"/>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E167"/>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E168"/>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E169"/>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E170"/>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E171"/>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E172"/>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E173"/>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E174"/>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E175"/>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E176"/>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E177"/>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E178"/>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E179"/>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E180"/>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E181"/>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E182"/>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E183"/>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E184"/>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E185"/>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E186"/>
     </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E187"/>
     </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E188"/>
     </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E189"/>
     </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E190"/>
     </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E191"/>
     </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E192"/>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E193"/>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E194"/>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E195"/>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E196"/>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E197"/>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E198"/>
     </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E199"/>
     </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E200"/>
     </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E201"/>
     </row>
-    <row r="202" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E202"/>
     </row>
-    <row r="203" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E203"/>
     </row>
-    <row r="204" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E204"/>
     </row>
-    <row r="205" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E205"/>
     </row>
-    <row r="206" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E206"/>
     </row>
-    <row r="207" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E207"/>
     </row>
-    <row r="208" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E208"/>
     </row>
-    <row r="209" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E209"/>
     </row>
-    <row r="210" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E210"/>
     </row>
-    <row r="211" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E211"/>
     </row>
-    <row r="212" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E212"/>
     </row>
-    <row r="213" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E213"/>
     </row>
-    <row r="214" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E214"/>
     </row>
-    <row r="215" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E215"/>
     </row>
-    <row r="216" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E216"/>
     </row>
-    <row r="217" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E217"/>
     </row>
-    <row r="218" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E218"/>
     </row>
-    <row r="219" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E219"/>
     </row>
-    <row r="220" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E220"/>
     </row>
-    <row r="221" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E221"/>
     </row>
-    <row r="222" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E222"/>
     </row>
-    <row r="223" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E223"/>
     </row>
-    <row r="224" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E224"/>
     </row>
-    <row r="225" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E225"/>
     </row>
-    <row r="226" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E226"/>
     </row>
-    <row r="227" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E227"/>
     </row>
-    <row r="228" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E228"/>
     </row>
-    <row r="229" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E229"/>
     </row>
-    <row r="230" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E230"/>
     </row>
-    <row r="231" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E231"/>
     </row>
-    <row r="232" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E232"/>
     </row>
-    <row r="233" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E233"/>
     </row>
-    <row r="234" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E234"/>
     </row>
-    <row r="235" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E235"/>
     </row>
-    <row r="236" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E236"/>
     </row>
-    <row r="237" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E237"/>
     </row>
-    <row r="238" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E238"/>
     </row>
-    <row r="239" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E239"/>
     </row>
-    <row r="240" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E240"/>
     </row>
-    <row r="241" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E241"/>
     </row>
-    <row r="242" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E242"/>
     </row>
-    <row r="243" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E243"/>
     </row>
-    <row r="244" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E244"/>
     </row>
-    <row r="245" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E245"/>
     </row>
-    <row r="246" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E246"/>
     </row>
-    <row r="247" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E247"/>
     </row>
-    <row r="248" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E248"/>
     </row>
-    <row r="249" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E249"/>
     </row>
-    <row r="250" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E250"/>
     </row>
-    <row r="251" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E251"/>
     </row>
-    <row r="252" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E252"/>
     </row>
-    <row r="253" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E253"/>
     </row>
-    <row r="254" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E254"/>
     </row>
-    <row r="255" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E255"/>
     </row>
-    <row r="256" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E256"/>
     </row>
-    <row r="257" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E257"/>
     </row>
-    <row r="258" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E258"/>
     </row>
-    <row r="259" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E259"/>
     </row>
-    <row r="260" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E260"/>
     </row>
-    <row r="261" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E261"/>
     </row>
-    <row r="262" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E262"/>
     </row>
-    <row r="263" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E263"/>
     </row>
-    <row r="264" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E264"/>
     </row>
-    <row r="265" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E265"/>
     </row>
-    <row r="266" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E266"/>
     </row>
-    <row r="267" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E267"/>
     </row>
-    <row r="268" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E268"/>
     </row>
-    <row r="269" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E269"/>
     </row>
-    <row r="270" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E270"/>
     </row>
-    <row r="271" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E271"/>
     </row>
-    <row r="272" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E272"/>
     </row>
-    <row r="273" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E273"/>
     </row>
-    <row r="274" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E274"/>
     </row>
-    <row r="275" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E275"/>
     </row>
-    <row r="276" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E276"/>
     </row>
-    <row r="277" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E277"/>
     </row>
-    <row r="278" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E278"/>
     </row>
-    <row r="279" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E279"/>
     </row>
-    <row r="280" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E280"/>
     </row>
-    <row r="281" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E281"/>
     </row>
-    <row r="282" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E282"/>
     </row>
-    <row r="283" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E283"/>
     </row>
-    <row r="284" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E284"/>
     </row>
-    <row r="285" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E285"/>
     </row>
-    <row r="286" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E286"/>
     </row>
-    <row r="287" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E287"/>
     </row>
-    <row r="288" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E288"/>
     </row>
-    <row r="289" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E289"/>
     </row>
-    <row r="290" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E290"/>
     </row>
-    <row r="291" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E291"/>
     </row>
-    <row r="292" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E292"/>
     </row>
-    <row r="293" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E293"/>
     </row>
-    <row r="294" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E294"/>
     </row>
-    <row r="295" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E295"/>
     </row>
-    <row r="296" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E296"/>
     </row>
-    <row r="297" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E297"/>
     </row>
-    <row r="298" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E298"/>
     </row>
-    <row r="299" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E299"/>
     </row>
-    <row r="300" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E300"/>
     </row>
-    <row r="301" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E301"/>
     </row>
-    <row r="302" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E302"/>
     </row>
-    <row r="303" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E303"/>
     </row>
-    <row r="304" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E304"/>
     </row>
-    <row r="305" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E305"/>
     </row>
-    <row r="306" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E306"/>
     </row>
-    <row r="307" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E307"/>
     </row>
-    <row r="308" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E308"/>
     </row>
-    <row r="309" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E309"/>
     </row>
-    <row r="310" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E310"/>
     </row>
-    <row r="311" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E311"/>
     </row>
-    <row r="312" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E312"/>
     </row>
-    <row r="313" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E313"/>
     </row>
-    <row r="314" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E314"/>
     </row>
-    <row r="315" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E315"/>
     </row>
-    <row r="316" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E316"/>
     </row>
-    <row r="317" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E317"/>
     </row>
-    <row r="318" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E318"/>
     </row>
-    <row r="319" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E319"/>
     </row>
-    <row r="320" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E320"/>
     </row>
-    <row r="321" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E321"/>
     </row>
-    <row r="322" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E322"/>
     </row>
-    <row r="323" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E323"/>
     </row>
-    <row r="324" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E324"/>
     </row>
-    <row r="325" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E325"/>
     </row>
-    <row r="326" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E326"/>
     </row>
-    <row r="327" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E327"/>
     </row>
-    <row r="328" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E328"/>
     </row>
-    <row r="329" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E329"/>
     </row>
-    <row r="330" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E330"/>
     </row>
-    <row r="331" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E331"/>
     </row>
-    <row r="332" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E332"/>
     </row>
-    <row r="333" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E333"/>
     </row>
-    <row r="334" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E334"/>
     </row>
-    <row r="335" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E335"/>
     </row>
-    <row r="336" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E336"/>
     </row>
-    <row r="337" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E337"/>
     </row>
-    <row r="338" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E338"/>
     </row>
-    <row r="339" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E339"/>
     </row>
-    <row r="340" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E340"/>
     </row>
-    <row r="341" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E341"/>
     </row>
-    <row r="342" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E342"/>
     </row>
-    <row r="343" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E343"/>
     </row>
-    <row r="344" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E344"/>
     </row>
-    <row r="345" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E345"/>
     </row>
-    <row r="346" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E346"/>
     </row>
-    <row r="347" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E347"/>
     </row>
-    <row r="348" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E348"/>
     </row>
-    <row r="349" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E349"/>
     </row>
-    <row r="350" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E350"/>
     </row>
-    <row r="351" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E351"/>
     </row>
-    <row r="352" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E352"/>
     </row>
-    <row r="353" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E353"/>
     </row>
-    <row r="354" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E354"/>
     </row>
-    <row r="355" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E355"/>
     </row>
-    <row r="356" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E356"/>
     </row>
-    <row r="357" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E357"/>
     </row>
-    <row r="358" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E358"/>
     </row>
-    <row r="359" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E359"/>
     </row>
-    <row r="360" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E360"/>
     </row>
-    <row r="361" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E361"/>
     </row>
-    <row r="362" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E362"/>
     </row>
-    <row r="363" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E363"/>
     </row>
-    <row r="364" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E364"/>
     </row>
-    <row r="365" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E365"/>
     </row>
-    <row r="366" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E366"/>
     </row>
-    <row r="367" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E367"/>
     </row>
-    <row r="368" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E368"/>
     </row>
-    <row r="369" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E369"/>
     </row>
-    <row r="370" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E370"/>
     </row>
-    <row r="371" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E371"/>
     </row>
-    <row r="372" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E372"/>
     </row>
-    <row r="373" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E373"/>
     </row>
-    <row r="374" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E374"/>
     </row>
-    <row r="375" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E375"/>
     </row>
-    <row r="376" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E376"/>
     </row>
-    <row r="377" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E377"/>
     </row>
-    <row r="378" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E378"/>
     </row>
-    <row r="379" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E379"/>
     </row>
-    <row r="380" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E380"/>
     </row>
-    <row r="381" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="381" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E381"/>
     </row>
-    <row r="382" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="382" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E382"/>
     </row>
-    <row r="383" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="383" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E383"/>
     </row>
-    <row r="384" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="384" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E384"/>
     </row>
-    <row r="385" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="385" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E385"/>
     </row>
-    <row r="386" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="386" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E386"/>
     </row>
-    <row r="387" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="387" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E387"/>
     </row>
-    <row r="388" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="388" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E388"/>
     </row>
-    <row r="389" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="389" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E389"/>
     </row>
-    <row r="390" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="390" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E390"/>
     </row>
-    <row r="391" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="391" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E391"/>
     </row>
-    <row r="392" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="392" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E392"/>
     </row>
-    <row r="393" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="393" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E393"/>
     </row>
-    <row r="394" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="394" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E394"/>
     </row>
-    <row r="395" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="395" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E395"/>
     </row>
-    <row r="396" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="396" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E396"/>
     </row>
-    <row r="397" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="397" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E397"/>
     </row>
-    <row r="398" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="398" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E398"/>
     </row>
-    <row r="399" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="399" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E399"/>
     </row>
-    <row r="400" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="400" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E400"/>
     </row>
-    <row r="401" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="401" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E401"/>
     </row>
-    <row r="402" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="402" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E402"/>
     </row>
-    <row r="403" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="403" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E403"/>
     </row>
-    <row r="404" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="404" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E404"/>
     </row>
-    <row r="405" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="405" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E405"/>
     </row>
-    <row r="406" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="406" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E406"/>
     </row>
-    <row r="407" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="407" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E407"/>
     </row>
-    <row r="408" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="408" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E408"/>
     </row>
-    <row r="409" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="409" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E409"/>
     </row>
-    <row r="410" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="410" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E410"/>
     </row>
-    <row r="411" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="411" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E411"/>
     </row>
-    <row r="412" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="412" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E412"/>
     </row>
-    <row r="413" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="413" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E413"/>
     </row>
-    <row r="414" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="414" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E414"/>
     </row>
-    <row r="415" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="415" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E415"/>
     </row>
-    <row r="416" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="416" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E416"/>
     </row>
-    <row r="417" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="417" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E417"/>
     </row>
-    <row r="418" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="418" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E418"/>
     </row>
-    <row r="419" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="419" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E419"/>
     </row>
-    <row r="420" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="420" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E420"/>
     </row>
-    <row r="421" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="421" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E421"/>
     </row>
-    <row r="422" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="422" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E422"/>
     </row>
-    <row r="423" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="423" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E423"/>
     </row>
-    <row r="424" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="424" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E424"/>
     </row>
-    <row r="425" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="425" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E425"/>
     </row>
-    <row r="426" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="426" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E426"/>
     </row>
-    <row r="427" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="427" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E427"/>
     </row>
-    <row r="428" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="428" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E428"/>
     </row>
-    <row r="429" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="429" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E429"/>
     </row>
-    <row r="430" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="430" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E430"/>
     </row>
-    <row r="431" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="431" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E431"/>
     </row>
-    <row r="432" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="432" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E432"/>
     </row>
-    <row r="433" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="433" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E433"/>
     </row>
-    <row r="434" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="434" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E434"/>
     </row>
-    <row r="435" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="435" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E435"/>
     </row>
-    <row r="436" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="436" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E436"/>
     </row>
-    <row r="437" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="437" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E437"/>
     </row>
-    <row r="438" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="438" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E438"/>
     </row>
-    <row r="439" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="439" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E439"/>
     </row>
-    <row r="440" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="440" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E440"/>
     </row>
-    <row r="441" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="441" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E441"/>
     </row>
-    <row r="442" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="442" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E442"/>
     </row>
-    <row r="443" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="443" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E443"/>
     </row>
-    <row r="444" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="444" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E444"/>
     </row>
-    <row r="445" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="445" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E445"/>
     </row>
-    <row r="446" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="446" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E446"/>
     </row>
-    <row r="447" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="447" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E447"/>
     </row>
-    <row r="448" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="448" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E448"/>
     </row>
-    <row r="449" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="449" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E449"/>
     </row>
-    <row r="450" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="450" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E450"/>
     </row>
-    <row r="451" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="451" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E451"/>
     </row>
-    <row r="452" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="452" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E452"/>
     </row>
-    <row r="453" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="453" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E453"/>
     </row>
-    <row r="454" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="454" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E454"/>
     </row>
-    <row r="455" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="455" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E455"/>
     </row>
-    <row r="456" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="456" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E456"/>
     </row>
-    <row r="457" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="457" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E457"/>
     </row>
-    <row r="458" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="458" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E458"/>
     </row>
-    <row r="459" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="459" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E459"/>
     </row>
-    <row r="460" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="460" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E460"/>
     </row>
-    <row r="461" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="461" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E461"/>
     </row>
-    <row r="462" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="462" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E462"/>
     </row>
-    <row r="463" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="463" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E463"/>
     </row>
-    <row r="464" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="464" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E464"/>
     </row>
-    <row r="465" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="465" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E465"/>
     </row>
-    <row r="466" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="466" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E466"/>
     </row>
-    <row r="467" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="467" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E467"/>
     </row>
-    <row r="468" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="468" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E468"/>
     </row>
-    <row r="469" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="469" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E469"/>
     </row>
-    <row r="470" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="470" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E470"/>
     </row>
-    <row r="471" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="471" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E471"/>
     </row>
-    <row r="472" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="472" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E472"/>
     </row>
-    <row r="473" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="473" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E473"/>
     </row>
-    <row r="474" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="474" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E474"/>
     </row>
-    <row r="475" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="475" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E475"/>
     </row>
-    <row r="476" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="476" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E476"/>
     </row>
-    <row r="477" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="477" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E477"/>
     </row>
-    <row r="478" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="478" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E478"/>
     </row>
-    <row r="479" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="479" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E479"/>
     </row>
-    <row r="480" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="480" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E480"/>
     </row>
-    <row r="481" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="481" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E481"/>
     </row>
-    <row r="482" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="482" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E482"/>
     </row>
-    <row r="483" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="483" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E483"/>
     </row>
-    <row r="484" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="484" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E484"/>
     </row>
-    <row r="485" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="485" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E485"/>
     </row>
-    <row r="486" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="486" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E486"/>
     </row>
-    <row r="487" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="487" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E487"/>
     </row>
-    <row r="488" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="488" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E488"/>
     </row>
-    <row r="489" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="489" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E489"/>
     </row>
-    <row r="490" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="490" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E490"/>
     </row>
-    <row r="491" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="491" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E491"/>
     </row>
-    <row r="492" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="492" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E492"/>
     </row>
-    <row r="493" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="493" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E493"/>
     </row>
-    <row r="494" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="494" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E494"/>
     </row>
-    <row r="495" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="495" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E495"/>
     </row>
-    <row r="496" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="496" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E496"/>
     </row>
-    <row r="497" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="497" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E497"/>
     </row>
-    <row r="498" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="498" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E498"/>
     </row>
-    <row r="499" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="499" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E499"/>
     </row>
-    <row r="500" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="500" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E500"/>
     </row>
-    <row r="501" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="501" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E501"/>
     </row>
-    <row r="502" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="502" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E502"/>
     </row>
-    <row r="503" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="503" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E503"/>
     </row>
-    <row r="504" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="504" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E504"/>
     </row>
-    <row r="505" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="505" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E505"/>
     </row>
   </sheetData>

</xml_diff>